<commit_message>
Changes after testing climber and calibrating shooter
</commit_message>
<xml_diff>
--- a/Documentation/ShooterLUTs/PracticeBot.xlsx
+++ b/Documentation/ShooterLUTs/PracticeBot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malep\Documents\GitHub\RapidReact\Documentation\ShooterLUTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0EF5AA1-A962-42A0-87E3-9C5940E465C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FD5679-D28F-4972-B50A-6CEE59DA3EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1130" yWindow="-110" windowWidth="21540" windowHeight="15260" xr2:uid="{0FB82E08-2372-48EE-B7C1-D25C920998DA}"/>
   </bookViews>
@@ -113,35 +113,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Distance</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs. Velocity</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -180,6 +151,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Velocity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -204,10 +186,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>8.1790000000000003</c:v>
                 </c:pt>
@@ -225,16 +207,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.2430000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.9344000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.359</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>11250</c:v>
                 </c:pt>
@@ -252,6 +240,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -259,7 +253,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C64E-464E-92A5-A0780CB9DF29}"/>
+              <c16:uniqueId val="{00000000-5926-4270-84A1-8FC7BAA72901}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -271,11 +265,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="591004527"/>
-        <c:axId val="591005359"/>
+        <c:axId val="409096160"/>
+        <c:axId val="409094912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591004527"/>
+        <c:axId val="409096160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -332,12 +326,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="591005359"/>
+        <c:crossAx val="409094912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591005359"/>
+        <c:axId val="409094912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -394,7 +388,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="591004527"/>
+        <c:crossAx val="409096160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1010,23 +1004,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1139825</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>212725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>517525</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EB1BAE4-40DE-4372-92D3-01255074CD73}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C25A10C-902F-4175-B979-4E2EAB6A2AAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1344,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D3E887-4936-491F-B95D-FAC7B794482F}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1432,6 +1426,28 @@
         <v>8800</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>7.9344000000000001</v>
+      </c>
+      <c r="C8">
+        <v>10700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>11.359</v>
+      </c>
+      <c r="C9">
+        <v>11250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update shooter LUT and pickup G path
</commit_message>
<xml_diff>
--- a/Documentation/ShooterLUTs/PracticeBot.xlsx
+++ b/Documentation/ShooterLUTs/PracticeBot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malep\Documents\GitHub\RapidReact\Documentation\ShooterLUTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FD5679-D28F-4972-B50A-6CEE59DA3EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2C792F-C71F-48E3-81D8-2C3A1D81B46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1130" yWindow="-110" windowWidth="21540" windowHeight="15260" xr2:uid="{0FB82E08-2372-48EE-B7C1-D25C920998DA}"/>
+    <workbookView xWindow="3050" yWindow="9550" windowWidth="15490" windowHeight="10510" xr2:uid="{0FB82E08-2372-48EE-B7C1-D25C920998DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,28 +191,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8.1790000000000003</c:v>
+                  <c:v>5.6029999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.6280000000000001</c:v>
+                  <c:v>7.298</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.1840000000000002</c:v>
+                  <c:v>7.9344000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3140000000000001</c:v>
+                  <c:v>10.342000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.7060000000000004</c:v>
+                  <c:v>11.598000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2430000000000003</c:v>
+                  <c:v>12.555999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.9344000000000001</c:v>
+                  <c:v>14.173999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.359</c:v>
+                  <c:v>16.925000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -224,28 +224,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>11250</c:v>
+                  <c:v>9250</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10000</c:v>
+                  <c:v>9750</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10000</c:v>
+                  <c:v>10650</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>11800</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9500</c:v>
+                  <c:v>12600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8800</c:v>
+                  <c:v>11800</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10700</c:v>
+                  <c:v>12250</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11250</c:v>
+                  <c:v>13100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1365,10 +1365,10 @@
         <v>60</v>
       </c>
       <c r="B2">
-        <v>8.1790000000000003</v>
+        <v>5.6029999999999998</v>
       </c>
       <c r="C2">
-        <v>11250</v>
+        <v>9250</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1376,10 +1376,10 @@
         <v>60</v>
       </c>
       <c r="B3">
-        <v>7.6280000000000001</v>
+        <v>7.298</v>
       </c>
       <c r="C3">
-        <v>10000</v>
+        <v>9750</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1387,10 +1387,10 @@
         <v>60</v>
       </c>
       <c r="B4">
-        <v>7.1840000000000002</v>
+        <v>7.9344000000000001</v>
       </c>
       <c r="C4">
-        <v>10000</v>
+        <v>10650</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1398,10 +1398,10 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>6.3140000000000001</v>
+        <v>10.342000000000001</v>
       </c>
       <c r="C5">
-        <v>10000</v>
+        <v>11800</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1409,10 +1409,10 @@
         <v>60</v>
       </c>
       <c r="B6">
-        <v>5.7060000000000004</v>
+        <v>11.598000000000001</v>
       </c>
       <c r="C6">
-        <v>9500</v>
+        <v>12600</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1420,10 +1420,10 @@
         <v>60</v>
       </c>
       <c r="B7">
-        <v>5.2430000000000003</v>
+        <v>12.555999999999999</v>
       </c>
       <c r="C7">
-        <v>8800</v>
+        <v>11800</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1431,10 +1431,10 @@
         <v>60</v>
       </c>
       <c r="B8">
-        <v>7.9344000000000001</v>
+        <v>14.173999999999999</v>
       </c>
       <c r="C8">
-        <v>10700</v>
+        <v>12250</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1442,10 +1442,10 @@
         <v>60</v>
       </c>
       <c r="B9">
-        <v>11.359</v>
+        <v>16.925000000000001</v>
       </c>
       <c r="C9">
-        <v>11250</v>
+        <v>13100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes after drive practice 3/9
</commit_message>
<xml_diff>
--- a/Documentation/ShooterLUTs/PracticeBot.xlsx
+++ b/Documentation/ShooterLUTs/PracticeBot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malep\Documents\GitHub\RapidReact\Documentation\ShooterLUTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2C792F-C71F-48E3-81D8-2C3A1D81B46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DBEAF2-1B2D-43AE-846B-9E4E825EC917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3050" yWindow="9550" windowWidth="15490" windowHeight="10510" xr2:uid="{0FB82E08-2372-48EE-B7C1-D25C920998DA}"/>
+    <workbookView xWindow="3050" yWindow="4530" windowWidth="15490" windowHeight="10510" xr2:uid="{0FB82E08-2372-48EE-B7C1-D25C920998DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -227,7 +227,7 @@
                   <c:v>9250</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9750</c:v>
+                  <c:v>10200</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10650</c:v>
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1379,7 +1379,7 @@
         <v>7.298</v>
       </c>
       <c r="C3">
-        <v>9750</v>
+        <v>10200</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add haptic feedback for when driver is not aligned
</commit_message>
<xml_diff>
--- a/Documentation/ShooterLUTs/PracticeBot.xlsx
+++ b/Documentation/ShooterLUTs/PracticeBot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malep\Documents\GitHub\RapidReact\Documentation\ShooterLUTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7638832B-C9B0-4596-AB00-CD22CEBE2FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52A42AF-E9F1-45A0-AA41-C09F76AD2A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1130" yWindow="-110" windowWidth="21540" windowHeight="15260" xr2:uid="{9A7BF167-04BC-4963-916B-4DC495AE685D}"/>
+    <workbookView xWindow="4800" yWindow="140" windowWidth="15490" windowHeight="10510" xr2:uid="{9A7BF167-04BC-4963-916B-4DC495AE685D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2306,7 +2306,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2416,15 +2416,15 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>10.657999999999999</v>
+        <v>6.3220000000000001</v>
       </c>
       <c r="B17">
         <f>0.3096*A17-2.1626</f>
-        <v>1.1371167999999998</v>
+        <v>-0.20530879999999985</v>
       </c>
       <c r="C17">
         <f>34.404*A17+8570.8</f>
-        <v>8937.4778319999987</v>
+        <v>8788.3020879999985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes after swerve module swap out
</commit_message>
<xml_diff>
--- a/Documentation/ShooterLUTs/PracticeBot.xlsx
+++ b/Documentation/ShooterLUTs/PracticeBot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malep\Documents\GitHub\RapidReact\Documentation\ShooterLUTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A9BFA3-0AD9-4F09-826C-C6123D656DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547F6C22-6D8D-4577-82E4-27B01E08B627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5330" yWindow="4530" windowWidth="15490" windowHeight="10510" xr2:uid="{9A7BF167-04BC-4963-916B-4DC495AE685D}"/>
+    <workbookView xWindow="1130" yWindow="-110" windowWidth="21540" windowHeight="15260" xr2:uid="{9A7BF167-04BC-4963-916B-4DC495AE685D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2416,15 +2416,15 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>8.9160000000000004</v>
+        <v>11.913</v>
       </c>
       <c r="B17">
         <f>0.27797*(A17-5.915)-0.6</f>
-        <v>0.23418797000000013</v>
+        <v>1.0672640599999998</v>
       </c>
       <c r="C17">
         <f>34.404*A17+8570.8</f>
-        <v>8877.5460640000001</v>
+        <v>8980.6548519999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes after calibrating shooter
</commit_message>
<xml_diff>
--- a/Documentation/ShooterLUTs/PracticeBot.xlsx
+++ b/Documentation/ShooterLUTs/PracticeBot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malep\Documents\GitHub\RapidReact\Documentation\ShooterLUTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AE9A47-29EE-42F8-A78E-475922032ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E10727-8274-48EA-8A07-CFD7D7234204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="5460" windowWidth="15490" windowHeight="10510" xr2:uid="{9A7BF167-04BC-4963-916B-4DC495AE685D}"/>
+    <workbookView xWindow="4100" yWindow="6410" windowWidth="15490" windowHeight="10510" xr2:uid="{9A7BF167-04BC-4963-916B-4DC495AE685D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,13 +56,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6897BB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,8 +91,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -119,36 +128,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Hood</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Angle vs. Distance</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -187,6 +166,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hood Angle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -211,60 +201,108 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>4.8129999999999997</c:v>
+                  <c:v>5.109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9059999999999997</c:v>
+                  <c:v>6.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.6612</c:v>
+                  <c:v>7.0209999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.1144999999999996</c:v>
+                  <c:v>8.1329999999999991</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.8190000000000008</c:v>
+                  <c:v>8.9489999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.7110000000000003</c:v>
+                  <c:v>9.8460000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.673999999999999</c:v>
+                  <c:v>10.930999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.917999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.747999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.920999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.827</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.648</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.358000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-0.67200000000000004</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.3</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.1</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.95</c:v>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -272,7 +310,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8543-4F37-8348-A3767F0DC38B}"/>
+              <c16:uniqueId val="{00000000-3C0A-4484-8A62-B8D3206C79A6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -284,11 +322,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1149550128"/>
-        <c:axId val="1149546800"/>
+        <c:axId val="1801429039"/>
+        <c:axId val="1801428207"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1149550128"/>
+        <c:axId val="1801429039"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -345,12 +383,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1149546800"/>
+        <c:crossAx val="1801428207"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1149546800"/>
+        <c:axId val="1801428207"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,7 +445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1149550128"/>
+        <c:crossAx val="1801429039"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -478,31 +516,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Velocity vs. Distance</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -541,6 +554,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Velocity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -565,60 +589,108 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>4.8129999999999997</c:v>
+                  <c:v>5.109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9059999999999997</c:v>
+                  <c:v>6.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.6612</c:v>
+                  <c:v>7.0209999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.1144999999999996</c:v>
+                  <c:v>8.1329999999999991</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.8190000000000008</c:v>
+                  <c:v>8.9489999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.7110000000000003</c:v>
+                  <c:v>9.8460000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.673999999999999</c:v>
+                  <c:v>10.930999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.917999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.747999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.920999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.827</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.648</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.358000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>Sheet1!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>8800</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8700</c:v>
+                  <c:v>8850</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8800</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8850</c:v>
+                  <c:v>9177</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8950</c:v>
+                  <c:v>9370</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9050</c:v>
+                  <c:v>9600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9275</c:v>
+                  <c:v>10050</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10679</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11390</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11718</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12403</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12938</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -626,7 +698,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-60E8-4A82-995B-6EECDFD36CE6}"/>
+              <c16:uniqueId val="{00000000-143D-48F6-B586-A2A33EDD9FE6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -638,11 +710,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1304981680"/>
-        <c:axId val="1304983344"/>
+        <c:axId val="1857152815"/>
+        <c:axId val="1857154063"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1304981680"/>
+        <c:axId val="1857152815"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,12 +771,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1304983344"/>
+        <c:crossAx val="1857154063"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1304983344"/>
+        <c:axId val="1857154063"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,7 +833,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1304981680"/>
+        <c:crossAx val="1857152815"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1933,23 +2005,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>606425</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>301625</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E23CD89-EA2D-4166-A193-9D6A07700C8F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22A5AFCD-A16D-4A6D-B0FA-F052A1F24C2D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1969,23 +2041,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>606425</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>187325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>301625</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>492125</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3B28C3D-6AD0-49B9-A95C-F0825C8B275E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25C3AA73-A0FD-4460-BFB1-0E096A62AF7D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2303,19 +2375,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DED074-4F02-4B1E-B2E8-932E9C2E5FA5}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="22.90625" customWidth="1"/>
     <col min="3" max="3" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2326,105 +2398,193 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>4.8129999999999997</v>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>5.109</v>
       </c>
       <c r="B2">
-        <v>-0.67200000000000004</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>8800</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>5.9059999999999997</v>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>6.08</v>
       </c>
       <c r="B3">
-        <v>-0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C3">
-        <v>8700</v>
+        <v>8850</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>6.6612</v>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>7.0209999999999999</v>
       </c>
       <c r="B4">
-        <v>-0.1</v>
+        <v>0.4</v>
       </c>
       <c r="C4">
-        <v>8800</v>
+        <v>9000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>8.1144999999999996</v>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>8.1329999999999991</v>
       </c>
       <c r="B5">
-        <v>0.35</v>
+        <v>0.7</v>
       </c>
       <c r="C5">
-        <v>8850</v>
+        <v>9177</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>8.8190000000000008</v>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>8.9489999999999998</v>
       </c>
       <c r="B6">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="C6">
-        <v>8950</v>
+        <v>9370</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>9.7110000000000003</v>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>9.8460000000000001</v>
       </c>
       <c r="B7">
+        <v>0.75</v>
+      </c>
+      <c r="C7">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>10.930999999999999</v>
+      </c>
+      <c r="B8">
+        <v>0.75</v>
+      </c>
+      <c r="C8">
+        <v>10050</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>11.917999999999999</v>
+      </c>
+      <c r="B9">
+        <v>0.75</v>
+      </c>
+      <c r="C9">
+        <v>10400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>12.843</v>
+      </c>
+      <c r="B10">
+        <v>0.75</v>
+      </c>
+      <c r="C10">
+        <v>10679</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>13.747999999999999</v>
+      </c>
+      <c r="B11">
         <v>0.9</v>
       </c>
-      <c r="C7">
-        <v>9050</v>
+      <c r="C11">
+        <v>11000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>10.673999999999999</v>
-      </c>
-      <c r="B8">
-        <v>0.95</v>
-      </c>
-      <c r="C8">
-        <v>9275</v>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>14.920999999999999</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>11390</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>15.827</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>11718</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>16.648</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>12403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>19.358000000000001</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>12938</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>3</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>8.6959999999999997</v>
-      </c>
-      <c r="B17">
-        <f>0.27797*(A17-5.915)-0.6</f>
-        <v>0.17303456999999989</v>
-      </c>
-      <c r="C17">
-        <f>34.404*A17+8570.8</f>
-        <v>8869.9771839999994</v>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>20.231999999999999</v>
+      </c>
+      <c r="B18">
+        <f>0.2092*(A18)-1.0698</f>
+        <v>3.1627343999999997</v>
+      </c>
+      <c r="C18">
+        <f>345.56*A18+6249</f>
+        <v>13240.369920000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes after field calibration
</commit_message>
<xml_diff>
--- a/Documentation/ShooterLUTs/PracticeBot.xlsx
+++ b/Documentation/ShooterLUTs/PracticeBot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malep\Documents\GitHub\RapidReact\Documentation\ShooterLUTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E10727-8274-48EA-8A07-CFD7D7234204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D64581-05A3-4E58-9472-3E02C785581F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="6410" windowWidth="15490" windowHeight="10510" xr2:uid="{9A7BF167-04BC-4963-916B-4DC495AE685D}"/>
+    <workbookView xWindow="1130" yWindow="-110" windowWidth="21540" windowHeight="15260" xr2:uid="{9A7BF167-04BC-4963-916B-4DC495AE685D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Distance</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Predicted velocity</t>
+  </si>
+  <si>
+    <t>Adjusted velocity</t>
   </si>
 </sst>
 </file>
@@ -201,64 +204,67 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$16</c:f>
+              <c:f>Sheet1!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>5.109</c:v>
+                  <c:v>5.1398739999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.08</c:v>
+                  <c:v>6.1108739999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0209999999999999</c:v>
+                  <c:v>7.0518739999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.1329999999999991</c:v>
+                  <c:v>8.1638739999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9489999999999998</c:v>
+                  <c:v>8.9798740000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.8460000000000001</c:v>
+                  <c:v>9.8768740000000008</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.930999999999999</c:v>
+                  <c:v>10.961874</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.917999999999999</c:v>
+                  <c:v>11.948874</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.843</c:v>
+                  <c:v>12.873874000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.747999999999999</c:v>
+                  <c:v>13.778874</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.920999999999999</c:v>
+                  <c:v>14.951874</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15.827</c:v>
+                  <c:v>15.857874000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.648</c:v>
+                  <c:v>16.678874</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.809999999999999</c:v>
+                  <c:v>17.840873999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19.358000000000001</c:v>
+                  <c:v>19.388874000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.253874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$16</c:f>
+              <c:f>Sheet1!$B$2:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -302,6 +308,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -310,7 +319,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3C0A-4484-8A62-B8D3206C79A6}"/>
+              <c16:uniqueId val="{00000000-1AAA-4019-B412-E3DAAFA59036}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -322,11 +331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1801429039"/>
-        <c:axId val="1801428207"/>
+        <c:axId val="1416110959"/>
+        <c:axId val="1416113871"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1801429039"/>
+        <c:axId val="1416110959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -383,12 +392,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1801428207"/>
+        <c:crossAx val="1416113871"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1801428207"/>
+        <c:axId val="1416113871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +454,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1801429039"/>
+        <c:crossAx val="1416110959"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -589,64 +598,67 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$16</c:f>
+              <c:f>Sheet1!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>5.109</c:v>
+                  <c:v>5.1398739999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.08</c:v>
+                  <c:v>6.1108739999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0209999999999999</c:v>
+                  <c:v>7.0518739999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.1329999999999991</c:v>
+                  <c:v>8.1638739999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9489999999999998</c:v>
+                  <c:v>8.9798740000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.8460000000000001</c:v>
+                  <c:v>9.8768740000000008</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.930999999999999</c:v>
+                  <c:v>10.961874</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.917999999999999</c:v>
+                  <c:v>11.948874</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.843</c:v>
+                  <c:v>12.873874000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.747999999999999</c:v>
+                  <c:v>13.778874</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.920999999999999</c:v>
+                  <c:v>14.951874</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15.827</c:v>
+                  <c:v>15.857874000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.648</c:v>
+                  <c:v>16.678874</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.809999999999999</c:v>
+                  <c:v>17.840873999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19.358000000000001</c:v>
+                  <c:v>19.388874000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.253874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$16</c:f>
+              <c:f>Sheet1!$C$2:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>8800</c:v>
                 </c:pt>
@@ -690,7 +702,10 @@
                   <c:v>12403</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12938</c:v>
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -698,7 +713,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-143D-48F6-B586-A2A33EDD9FE6}"/>
+              <c16:uniqueId val="{00000000-C2EA-41F9-871E-E4987C77B9F1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -710,11 +725,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1857152815"/>
-        <c:axId val="1857154063"/>
+        <c:axId val="1416137999"/>
+        <c:axId val="1416138415"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1857152815"/>
+        <c:axId val="1416137999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,12 +786,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1857154063"/>
+        <c:crossAx val="1416138415"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1857154063"/>
+        <c:axId val="1416138415"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,7 +848,401 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1857152815"/>
+        <c:crossAx val="1416137999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adjusted velocity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>5.1398739999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1108739999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0518739999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1638739999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9798740000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8768740000000008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.961874</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.948874</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.873874000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.778874</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.951874</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.857874000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.678874</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.840873999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.388874000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.253874</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>8999.999976000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9051.1363395000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9204.5454300000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9385.568156790001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9582.9545199000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9818.1817920000012</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10278.409063500001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10636.363608000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10921.704516330001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11249.999970000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11648.863605300001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11984.318149860001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12273.749967270001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12684.88632981</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13295.454510000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13653.409054500002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2A90-48AB-B4EC-B75ED38DE34A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1279201023"/>
+        <c:axId val="1279202271"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1279201023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1279202271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1279202271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1279201023"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -969,6 +1378,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2001,27 +2450,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22A5AFCD-A16D-4A6D-B0FA-F052A1F24C2D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49173FEF-3A8A-4EC7-BA74-605F173C5C47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2041,23 +3006,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>187325</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>492125</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25C3AA73-A0FD-4460-BFB1-0E096A62AF7D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{530F2069-28A8-45E5-A9F7-8629E2CDD87B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2070,6 +3035,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F7FBFB2-2480-4AEC-A5C3-5E931C05F3A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2375,19 +3376,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DED074-4F02-4B1E-B2E8-932E9C2E5FA5}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="22.90625" customWidth="1"/>
     <col min="3" max="3" width="27.26953125" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2397,10 +3399,13 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>5.109</v>
+        <v>5.1398739999999998</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2408,10 +3413,14 @@
       <c r="C2">
         <v>8800</v>
       </c>
+      <c r="D2">
+        <f>C2*1.02272727</f>
+        <v>8999.999976000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>6.08</v>
+        <v>6.1108739999999999</v>
       </c>
       <c r="B3">
         <v>0.2</v>
@@ -2419,10 +3428,14 @@
       <c r="C3">
         <v>8850</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D17" si="0">C3*1.02272727</f>
+        <v>9051.1363395000008</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>7.0209999999999999</v>
+        <v>7.0518739999999998</v>
       </c>
       <c r="B4">
         <v>0.4</v>
@@ -2430,10 +3443,14 @@
       <c r="C4">
         <v>9000</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>9204.5454300000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>8.1329999999999991</v>
+        <v>8.1638739999999999</v>
       </c>
       <c r="B5">
         <v>0.7</v>
@@ -2441,10 +3458,14 @@
       <c r="C5">
         <v>9177</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>9385.568156790001</v>
+      </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>8.9489999999999998</v>
+        <v>8.9798740000000006</v>
       </c>
       <c r="B6">
         <v>0.75</v>
@@ -2452,10 +3473,14 @@
       <c r="C6">
         <v>9370</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>9582.9545199000004</v>
+      </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>9.8460000000000001</v>
+        <v>9.8768740000000008</v>
       </c>
       <c r="B7">
         <v>0.75</v>
@@ -2463,10 +3488,14 @@
       <c r="C7">
         <v>9600</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>9818.1817920000012</v>
+      </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>10.930999999999999</v>
+        <v>10.961874</v>
       </c>
       <c r="B8">
         <v>0.75</v>
@@ -2474,10 +3503,14 @@
       <c r="C8">
         <v>10050</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>10278.409063500001</v>
+      </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>11.917999999999999</v>
+        <v>11.948874</v>
       </c>
       <c r="B9">
         <v>0.75</v>
@@ -2485,10 +3518,14 @@
       <c r="C9">
         <v>10400</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>10636.363608000001</v>
+      </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>12.843</v>
+        <v>12.873874000000001</v>
       </c>
       <c r="B10">
         <v>0.75</v>
@@ -2496,10 +3533,14 @@
       <c r="C10">
         <v>10679</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>10921.704516330001</v>
+      </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>13.747999999999999</v>
+        <v>13.778874</v>
       </c>
       <c r="B11">
         <v>0.9</v>
@@ -2507,10 +3548,14 @@
       <c r="C11">
         <v>11000</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>11249.999970000001</v>
+      </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>14.920999999999999</v>
+        <v>14.951874</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2518,10 +3563,14 @@
       <c r="C12">
         <v>11390</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>11648.863605300001</v>
+      </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>15.827</v>
+        <v>15.857874000000001</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2529,10 +3578,14 @@
       <c r="C13">
         <v>11718</v>
       </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>11984.318149860001</v>
+      </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>16.648</v>
+        <v>16.678874</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2540,10 +3593,14 @@
       <c r="C14">
         <v>12001</v>
       </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>12273.749967270001</v>
+      </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>17.809999999999999</v>
+        <v>17.840873999999999</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2551,39 +3608,62 @@
       <c r="C15">
         <v>12403</v>
       </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>12684.88632981</v>
+      </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>19.358000000000001</v>
+        <v>19.388874000000001</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>12938</v>
+        <v>13000</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>13295.454510000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>20.253874</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>13350</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>13653.409054500002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>3</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1">
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
         <v>20.231999999999999</v>
       </c>
-      <c r="B18">
-        <f>0.2092*(A18)-1.0698</f>
+      <c r="B19">
+        <f>0.2092*(A19)-1.0698</f>
         <v>3.1627343999999997</v>
       </c>
-      <c r="C18">
-        <f>345.56*A18+6249</f>
+      <c r="C19">
+        <f>345.56*A19+6249</f>
         <v>13240.369920000001</v>
       </c>
     </row>

</xml_diff>